<commit_message>
Rates and Records deletion before upload
</commit_message>
<xml_diff>
--- a/Web/UserEx.Web/wwwroot/Files/CDRs-05_11_09_2022-58.xlsx
+++ b/Web/UserEx.Web/wwwroot/Files/CDRs-05_11_09_2022-58.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:40009_{FE1188AE-CE64-4C70-85CC-BE83470E41A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA3C170F-52D9-47E0-A728-D6EDBC0FC023}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="0" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CDRs-05_11_09_2022-58" sheetId="1" r:id="rId1"/>
@@ -932,8 +932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G591"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="A304" workbookViewId="0">
+      <selection activeCell="G318" sqref="G318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>